<commit_message>
add xlsx settings fixed AI In.Imit_Mode string add No Tag Name warning
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kek\PycharmProjects\RSLogix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B2289C-9C6C-4808-8FF5-1C47E58E8C1B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EE1C3E-3780-4FF8-BF30-CEF1178227C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15135" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10485" yWindow="3240" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1539,8 +1549,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1622,7 +1632,7 @@
       </c>
       <c r="B2" s="2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>VRJERV</v>
+        <v>XMHDCO</v>
       </c>
       <c r="C2" t="s">
         <v>332</v>
@@ -1658,7 +1668,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" ref="B4:B63" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>SJLDXS</v>
+        <v>GTQLBU</v>
       </c>
       <c r="C4" t="s">
         <v>337</v>
@@ -1692,10 +1702,7 @@
       <c r="A6" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B6" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>WFUKUO</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
         <v>339</v>
       </c>
@@ -1728,10 +1735,7 @@
       <c r="A8" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B8" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>QBJLKC</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" t="s">
         <v>341</v>
       </c>
@@ -1764,10 +1768,7 @@
       <c r="A10" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B10" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>RJQNFV</v>
-      </c>
+      <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>343</v>
       </c>
@@ -1800,10 +1801,7 @@
       <c r="A12" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B12" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>GBAYHP</v>
-      </c>
+      <c r="B12" s="2"/>
       <c r="C12" t="s">
         <v>347</v>
       </c>
@@ -1836,10 +1834,7 @@
       <c r="A14" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B14" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>QQFBFJ</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="C14" t="s">
         <v>351</v>
       </c>
@@ -1872,10 +1867,7 @@
       <c r="A16" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B16" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>VRCSMN</v>
-      </c>
+      <c r="B16" s="2"/>
       <c r="C16" t="s">
         <v>355</v>
       </c>
@@ -1938,7 +1930,7 @@
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>FJJXET</v>
+        <v>MGBMID</v>
       </c>
       <c r="C21" t="s">
         <v>360</v>
@@ -1974,7 +1966,7 @@
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>CLOJWX</v>
+        <v>PZWCFO</v>
       </c>
       <c r="C23" t="s">
         <v>362</v>
@@ -2010,7 +2002,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LMGTIM</v>
+        <v>BJLIDE</v>
       </c>
       <c r="C25" t="s">
         <v>364</v>
@@ -2046,7 +2038,7 @@
       </c>
       <c r="B27" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>OTFGFB</v>
+        <v>YMSLOP</v>
       </c>
       <c r="C27" t="s">
         <v>366</v>
@@ -2082,7 +2074,7 @@
       </c>
       <c r="B29" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WRPRFX</v>
+        <v>GATSNU</v>
       </c>
       <c r="C29" t="s">
         <v>368</v>
@@ -2118,7 +2110,7 @@
       </c>
       <c r="B31" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>STSOEA</v>
+        <v>BQSCYY</v>
       </c>
       <c r="C31" t="s">
         <v>370</v>
@@ -2160,7 +2152,7 @@
       </c>
       <c r="B33" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>YABBYC</v>
+        <v>HQYUPV</v>
       </c>
       <c r="C33" t="s">
         <v>375</v>
@@ -2193,7 +2185,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DRANKJ</v>
+        <v>SXHQPN</v>
       </c>
       <c r="C35" t="s">
         <v>376</v>
@@ -2278,7 +2270,7 @@
       </c>
       <c r="B42" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NPDNJX</v>
+        <v>TAZMPN</v>
       </c>
       <c r="C42" t="s">
         <v>252</v>
@@ -2302,7 +2294,7 @@
       </c>
       <c r="B43" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>IXJNKC</v>
+        <v>WUECTU</v>
       </c>
       <c r="D43" t="s">
         <v>257</v>
@@ -2317,7 +2309,7 @@
       </c>
       <c r="B44" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>QLNZAH</v>
+        <v>MBXYPM</v>
       </c>
       <c r="D44" t="s">
         <v>259</v>
@@ -2332,7 +2324,7 @@
       </c>
       <c r="B45" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ZUWGGL</v>
+        <v>OPPBUR</v>
       </c>
       <c r="C45" t="s">
         <v>261</v>
@@ -2377,7 +2369,7 @@
       </c>
       <c r="B48" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>TPNHHS</v>
+        <v>HJEXQN</v>
       </c>
       <c r="C48" t="s">
         <v>267</v>
@@ -2434,7 +2426,7 @@
       </c>
       <c r="B52" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ADZKFI</v>
+        <v>VZJXOE</v>
       </c>
       <c r="C52" t="s">
         <v>271</v>
@@ -2495,7 +2487,7 @@
       </c>
       <c r="B57" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>YECORK</v>
+        <v>DFASJC</v>
       </c>
       <c r="C57" t="s">
         <v>273</v>
@@ -2540,7 +2532,7 @@
       </c>
       <c r="B60" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>EOSEBM</v>
+        <v>ZAGWXK</v>
       </c>
       <c r="C60" t="s">
         <v>274</v>
@@ -2585,7 +2577,7 @@
       </c>
       <c r="B63" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>TRIGMU</v>
+        <v>MEMLFH</v>
       </c>
       <c r="C63" t="s">
         <v>275</v>
@@ -2642,7 +2634,7 @@
       </c>
       <c r="B67" s="2" t="str">
         <f t="shared" ref="B67:B130" ca="1" si="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>HNCZUK</v>
+        <v>RUPRIB</v>
       </c>
       <c r="C67" t="s">
         <v>276</v>
@@ -2679,7 +2671,7 @@
       </c>
       <c r="B70" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FWIDGF</v>
+        <v>LSQGZU</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>10</v>
@@ -2706,7 +2698,7 @@
       </c>
       <c r="B71" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>YHHYYK</v>
+        <v>PHBLOO</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>17</v>
@@ -2733,7 +2725,7 @@
       </c>
       <c r="B72" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FQXMIZ</v>
+        <v>VVTXPY</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>23</v>
@@ -2760,7 +2752,7 @@
       </c>
       <c r="B73" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WGKUUK</v>
+        <v>BKRGYH</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>27</v>
@@ -2787,7 +2779,7 @@
       </c>
       <c r="B74" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QRAOKE</v>
+        <v>COKYOB</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>33</v>
@@ -2814,7 +2806,7 @@
       </c>
       <c r="B75" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CVPEIN</v>
+        <v>JDRHBD</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>37</v>
@@ -2841,7 +2833,7 @@
       </c>
       <c r="B76" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BUNEBC</v>
+        <v>HAMIDS</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>41</v>
@@ -2865,7 +2857,7 @@
       </c>
       <c r="B77" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OFOKIZ</v>
+        <v>WAPGQM</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>46</v>
@@ -2892,7 +2884,7 @@
       </c>
       <c r="B78" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BBROES</v>
+        <v>XUWFSB</v>
       </c>
       <c r="C78" t="s">
         <v>138</v>
@@ -2919,7 +2911,7 @@
       </c>
       <c r="B79" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QGDJPZ</v>
+        <v>NGTSHU</v>
       </c>
       <c r="C79" t="s">
         <v>140</v>
@@ -2946,7 +2938,7 @@
       </c>
       <c r="B80" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QISUUP</v>
+        <v>GVNSQE</v>
       </c>
       <c r="C80" t="s">
         <v>142</v>
@@ -2973,7 +2965,7 @@
       </c>
       <c r="B81" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAJEZC</v>
+        <v>UFLXOM</v>
       </c>
       <c r="C81" t="s">
         <v>144</v>
@@ -2997,7 +2989,7 @@
       </c>
       <c r="B82" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WLUCKQ</v>
+        <v>VOOACM</v>
       </c>
       <c r="C82" t="s">
         <v>147</v>
@@ -3018,7 +3010,7 @@
       </c>
       <c r="B83" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IFQMDT</v>
+        <v>JULOUS</v>
       </c>
       <c r="C83" t="s">
         <v>148</v>
@@ -3045,7 +3037,7 @@
       </c>
       <c r="B84" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZEWGBU</v>
+        <v>LBMTYJ</v>
       </c>
       <c r="C84" t="s">
         <v>152</v>
@@ -3072,7 +3064,7 @@
       </c>
       <c r="B85" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CIPKND</v>
+        <v>TKAHFW</v>
       </c>
       <c r="C85" t="s">
         <v>154</v>
@@ -3106,7 +3098,7 @@
       </c>
       <c r="B87" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KJUZIO</v>
+        <v>ZCZNPS</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>51</v>
@@ -3127,7 +3119,7 @@
       </c>
       <c r="B88" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZPECUS</v>
+        <v>BVPRPY</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>53</v>
@@ -3154,7 +3146,7 @@
       </c>
       <c r="B89" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SERUFC</v>
+        <v>ABVQQP</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>57</v>
@@ -3181,7 +3173,7 @@
       </c>
       <c r="B90" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JCTTLX</v>
+        <v>CILYNR</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>60</v>
@@ -3205,7 +3197,7 @@
       </c>
       <c r="B91" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZQLVJY</v>
+        <v>BXQCZD</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>63</v>
@@ -3229,7 +3221,7 @@
       </c>
       <c r="B92" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DGZZSA</v>
+        <v>FHZIGI</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>65</v>
@@ -3253,7 +3245,7 @@
       </c>
       <c r="B93" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XUOQXX</v>
+        <v>HXQMWL</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>68</v>
@@ -3277,7 +3269,7 @@
       </c>
       <c r="B94" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WDCJIX</v>
+        <v>VEHMOP</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>70</v>
@@ -3301,7 +3293,7 @@
       </c>
       <c r="B95" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SEUVAB</v>
+        <v>INREMB</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>73</v>
@@ -3325,7 +3317,7 @@
       </c>
       <c r="B96" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LIWEZT</v>
+        <v>IKEXJS</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>77</v>
@@ -3349,7 +3341,7 @@
       </c>
       <c r="B97" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VGDNUN</v>
+        <v>BFSEXX</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>81</v>
@@ -3373,7 +3365,7 @@
       </c>
       <c r="B98" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JXQXBP</v>
+        <v>CLGBSA</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>85</v>
@@ -3397,7 +3389,7 @@
       </c>
       <c r="B99" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FPIMUE</v>
+        <v>GQETJU</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>89</v>
@@ -3421,7 +3413,7 @@
       </c>
       <c r="B100" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BTSFHQ</v>
+        <v>JHKAJZ</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>93</v>
@@ -3448,7 +3440,7 @@
       </c>
       <c r="B101" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DUSZFC</v>
+        <v>LIBIVB</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>99</v>
@@ -3478,7 +3470,7 @@
       </c>
       <c r="B102" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FHZACI</v>
+        <v>BRETEF</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>106</v>
@@ -3513,7 +3505,7 @@
       </c>
       <c r="B104" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XVYYJP</v>
+        <v>RMNRTG</v>
       </c>
       <c r="C104" t="s">
         <v>114</v>
@@ -3537,7 +3529,7 @@
       </c>
       <c r="B105" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NBCFOV</v>
+        <v>TDEMSK</v>
       </c>
       <c r="C105" t="s">
         <v>117</v>
@@ -3561,7 +3553,7 @@
       </c>
       <c r="B106" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IRJRJI</v>
+        <v>VDJTHW</v>
       </c>
       <c r="C106" t="s">
         <v>120</v>
@@ -3585,7 +3577,7 @@
       </c>
       <c r="B107" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VQWMVE</v>
+        <v>DXACVQ</v>
       </c>
       <c r="C107" t="s">
         <v>123</v>
@@ -3609,7 +3601,7 @@
       </c>
       <c r="B108" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WWRSTW</v>
+        <v>XILBQY</v>
       </c>
       <c r="C108" t="s">
         <v>126</v>
@@ -3633,7 +3625,7 @@
       </c>
       <c r="B109" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GBINKF</v>
+        <v>GHECNY</v>
       </c>
       <c r="C109" t="s">
         <v>129</v>
@@ -3657,7 +3649,7 @@
       </c>
       <c r="B110" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GBOMKL</v>
+        <v>KGWQYZ</v>
       </c>
       <c r="C110" t="s">
         <v>132</v>
@@ -3681,7 +3673,7 @@
       </c>
       <c r="B111" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>EJBSYT</v>
+        <v>HNRZXF</v>
       </c>
       <c r="C111" t="s">
         <v>135</v>
@@ -3705,7 +3697,7 @@
       </c>
       <c r="B112" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NKAEPT</v>
+        <v>GPIAQL</v>
       </c>
       <c r="C112" t="s">
         <v>158</v>
@@ -3732,7 +3724,7 @@
       </c>
       <c r="B113" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DOCLKT</v>
+        <v>HZMSJS</v>
       </c>
       <c r="C113" t="s">
         <v>162</v>
@@ -3759,7 +3751,7 @@
       </c>
       <c r="B114" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SPDXAT</v>
+        <v>RFGQLA</v>
       </c>
       <c r="C114" t="s">
         <v>164</v>
@@ -3786,7 +3778,7 @@
       </c>
       <c r="B115" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HZSVXD</v>
+        <v>ZKYBXN</v>
       </c>
       <c r="C115" t="s">
         <v>168</v>
@@ -3807,7 +3799,7 @@
       </c>
       <c r="B116" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CDOTKU</v>
+        <v>VPPRNO</v>
       </c>
       <c r="C116" t="s">
         <v>169</v>
@@ -3834,7 +3826,7 @@
       </c>
       <c r="B117" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>STYESC</v>
+        <v>LBATSL</v>
       </c>
       <c r="C117" t="s">
         <v>171</v>
@@ -3855,7 +3847,7 @@
       </c>
       <c r="B118" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BGSQEJ</v>
+        <v>OPZSAF</v>
       </c>
       <c r="C118" t="s">
         <v>172</v>
@@ -3876,7 +3868,7 @@
       </c>
       <c r="B119" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QIGEUF</v>
+        <v>QBHCCV</v>
       </c>
       <c r="C119" t="s">
         <v>173</v>
@@ -3904,7 +3896,7 @@
       </c>
       <c r="B121" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PASWCL</v>
+        <v>HYLLFY</v>
       </c>
       <c r="C121" t="s">
         <v>278</v>
@@ -3928,7 +3920,7 @@
       </c>
       <c r="B122" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GOTUIN</v>
+        <v>CQJTSW</v>
       </c>
       <c r="C122" t="s">
         <v>281</v>
@@ -3952,7 +3944,7 @@
       </c>
       <c r="B123" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FHUSGR</v>
+        <v>ULHQPR</v>
       </c>
       <c r="C123" t="s">
         <v>284</v>
@@ -3976,7 +3968,7 @@
       </c>
       <c r="B124" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KKHNEZ</v>
+        <v>HIZTDM</v>
       </c>
       <c r="C124" t="s">
         <v>287</v>
@@ -4000,7 +3992,7 @@
       </c>
       <c r="B125" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DRPODK</v>
+        <v>IWVOUK</v>
       </c>
       <c r="C125" t="s">
         <v>290</v>
@@ -4024,7 +4016,7 @@
       </c>
       <c r="B126" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NNPXKC</v>
+        <v>YZHPZP</v>
       </c>
       <c r="C126" t="s">
         <v>292</v>
@@ -4048,7 +4040,7 @@
       </c>
       <c r="B127" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GBZZDC</v>
+        <v>VBZCBP</v>
       </c>
       <c r="C127" t="s">
         <v>294</v>
@@ -4072,7 +4064,7 @@
       </c>
       <c r="B128" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GNFZDW</v>
+        <v>YKEFCZ</v>
       </c>
       <c r="C128" t="s">
         <v>296</v>
@@ -4096,7 +4088,7 @@
       </c>
       <c r="B129" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SMIVHQ</v>
+        <v>QNBRST</v>
       </c>
       <c r="C129" t="s">
         <v>298</v>
@@ -4120,7 +4112,7 @@
       </c>
       <c r="B130" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LCZMZM</v>
+        <v>EOWHGO</v>
       </c>
       <c r="C130" t="s">
         <v>300</v>
@@ -4144,7 +4136,7 @@
       </c>
       <c r="B131" s="2" t="str">
         <f t="shared" ref="B131:B187" ca="1" si="2">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>DYSLBI</v>
+        <v>WDAJPW</v>
       </c>
       <c r="C131" t="s">
         <v>302</v>
@@ -4168,7 +4160,7 @@
       </c>
       <c r="B132" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ICBQHY</v>
+        <v>HZHELH</v>
       </c>
       <c r="C132" t="s">
         <v>304</v>
@@ -4192,7 +4184,7 @@
       </c>
       <c r="B133" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NBEZZP</v>
+        <v>NRDYZQ</v>
       </c>
       <c r="C133" t="s">
         <v>306</v>
@@ -4216,7 +4208,7 @@
       </c>
       <c r="B134" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LEBIQO</v>
+        <v>WBBJZY</v>
       </c>
       <c r="C134" t="s">
         <v>308</v>
@@ -4240,7 +4232,7 @@
       </c>
       <c r="B135" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DYZXUK</v>
+        <v>WEQLCL</v>
       </c>
       <c r="C135" t="s">
         <v>309</v>
@@ -4264,7 +4256,7 @@
       </c>
       <c r="B136" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GSIXAL</v>
+        <v>EICODP</v>
       </c>
       <c r="C136" t="s">
         <v>310</v>
@@ -4292,7 +4284,7 @@
       </c>
       <c r="B138" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UIGKFF</v>
+        <v>NUAVWM</v>
       </c>
       <c r="C138" t="s">
         <v>312</v>
@@ -4316,7 +4308,7 @@
       </c>
       <c r="B139" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TUCYPW</v>
+        <v>RFTCPP</v>
       </c>
       <c r="C139" t="s">
         <v>313</v>
@@ -4340,7 +4332,7 @@
       </c>
       <c r="B140" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SGRLHF</v>
+        <v>HFWDNA</v>
       </c>
       <c r="C140" t="s">
         <v>314</v>
@@ -4364,7 +4356,7 @@
       </c>
       <c r="B141" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KFMTDV</v>
+        <v>YBUKUE</v>
       </c>
       <c r="C141" t="s">
         <v>315</v>
@@ -4388,7 +4380,7 @@
       </c>
       <c r="B142" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MAFRDC</v>
+        <v>TNOHFS</v>
       </c>
       <c r="C142" t="s">
         <v>316</v>
@@ -4412,7 +4404,7 @@
       </c>
       <c r="B143" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AYUQWV</v>
+        <v>LVAFZQ</v>
       </c>
       <c r="C143" t="s">
         <v>317</v>
@@ -4436,7 +4428,7 @@
       </c>
       <c r="B144" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KOBXZZ</v>
+        <v>HQNNPT</v>
       </c>
       <c r="C144" t="s">
         <v>319</v>
@@ -4460,7 +4452,7 @@
       </c>
       <c r="B145" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BSPGXO</v>
+        <v>LCVEIY</v>
       </c>
       <c r="C145" t="s">
         <v>321</v>
@@ -4484,7 +4476,7 @@
       </c>
       <c r="B146" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VLJDXC</v>
+        <v>JBHUJX</v>
       </c>
       <c r="C146" t="s">
         <v>377</v>
@@ -4508,7 +4500,7 @@
       </c>
       <c r="B147" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GMGQQG</v>
+        <v>QKLTAO</v>
       </c>
       <c r="C147" t="s">
         <v>379</v>
@@ -4529,7 +4521,7 @@
       </c>
       <c r="B148" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UULRWJ</v>
+        <v>IOEICW</v>
       </c>
       <c r="C148" t="s">
         <v>381</v>
@@ -4550,7 +4542,7 @@
       </c>
       <c r="B149" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCDDKR</v>
+        <v>HSVDRP</v>
       </c>
       <c r="C149" t="s">
         <v>382</v>
@@ -4571,7 +4563,7 @@
       </c>
       <c r="B150" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LWASVN</v>
+        <v>DJUMYY</v>
       </c>
       <c r="C150" t="s">
         <v>383</v>
@@ -4592,7 +4584,7 @@
       </c>
       <c r="B151" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>IZSJRJ</v>
+        <v>FMZJFL</v>
       </c>
       <c r="C151" t="s">
         <v>384</v>
@@ -4613,7 +4605,7 @@
       </c>
       <c r="B152" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NIHBHG</v>
+        <v>CWOONP</v>
       </c>
       <c r="C152" t="s">
         <v>385</v>
@@ -4634,7 +4626,7 @@
       </c>
       <c r="B153" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YCNTBF</v>
+        <v>RYZPBK</v>
       </c>
       <c r="C153" t="s">
         <v>386</v>
@@ -4659,7 +4651,7 @@
       </c>
       <c r="B155" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GSSCPA</v>
+        <v>YZNULD</v>
       </c>
       <c r="C155" t="s">
         <v>177</v>
@@ -4689,7 +4681,7 @@
       </c>
       <c r="B156" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HNKCCL</v>
+        <v>OOPKOA</v>
       </c>
       <c r="C156" t="s">
         <v>183</v>
@@ -4716,7 +4708,7 @@
       </c>
       <c r="B157" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NYXKSG</v>
+        <v>HBYDHD</v>
       </c>
       <c r="C157" t="s">
         <v>188</v>
@@ -4743,7 +4735,7 @@
       </c>
       <c r="B158" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VUOGPS</v>
+        <v>HPSPXC</v>
       </c>
       <c r="C158" t="s">
         <v>192</v>
@@ -4770,7 +4762,7 @@
       </c>
       <c r="B159" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JMUUDB</v>
+        <v>TTCMVV</v>
       </c>
       <c r="C159" t="s">
         <v>196</v>
@@ -4797,7 +4789,7 @@
       </c>
       <c r="B160" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KAUNNI</v>
+        <v>NRSCIN</v>
       </c>
       <c r="C160" t="s">
         <v>200</v>
@@ -4824,7 +4816,7 @@
       </c>
       <c r="B161" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TBCRBJ</v>
+        <v>EPMRUY</v>
       </c>
       <c r="C161" t="s">
         <v>204</v>
@@ -4845,7 +4837,7 @@
       </c>
       <c r="B162" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VBKBIJ</v>
+        <v>PFPVCC</v>
       </c>
       <c r="C162" t="s">
         <v>207</v>
@@ -4866,7 +4858,7 @@
       </c>
       <c r="B163" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PJJTOB</v>
+        <v>NDGMLP</v>
       </c>
       <c r="C163" t="s">
         <v>210</v>
@@ -4887,7 +4879,7 @@
       </c>
       <c r="B164" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YYHFTY</v>
+        <v>QMQJJR</v>
       </c>
       <c r="C164" t="s">
         <v>213</v>
@@ -4908,7 +4900,7 @@
       </c>
       <c r="B165" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WNZDHH</v>
+        <v>FATZIB</v>
       </c>
       <c r="C165" t="s">
         <v>216</v>
@@ -4929,7 +4921,7 @@
       </c>
       <c r="B166" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PCYNGU</v>
+        <v>RWHSMY</v>
       </c>
       <c r="C166" t="s">
         <v>219</v>
@@ -4950,7 +4942,7 @@
       </c>
       <c r="B167" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JWLURE</v>
+        <v>XJMXPT</v>
       </c>
       <c r="C167" t="s">
         <v>222</v>
@@ -4971,7 +4963,7 @@
       </c>
       <c r="B168" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TKDREX</v>
+        <v>PUXSZK</v>
       </c>
       <c r="C168" t="s">
         <v>224</v>
@@ -4992,7 +4984,7 @@
       </c>
       <c r="B169" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QYIYNV</v>
+        <v>FEJJMC</v>
       </c>
       <c r="C169" t="s">
         <v>226</v>
@@ -5016,7 +5008,7 @@
       </c>
       <c r="B170" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XHDVQD</v>
+        <v>KGCANG</v>
       </c>
       <c r="C170" t="s">
         <v>229</v>
@@ -5044,7 +5036,7 @@
       </c>
       <c r="B172" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>EIKNYP</v>
+        <v>VDDUWL</v>
       </c>
       <c r="C172" t="s">
         <v>232</v>
@@ -5068,7 +5060,7 @@
       </c>
       <c r="B173" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PTESRE</v>
+        <v>ULLRJF</v>
       </c>
       <c r="C173" t="s">
         <v>233</v>
@@ -5092,7 +5084,7 @@
       </c>
       <c r="B174" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OBUVSF</v>
+        <v>XAEQIJ</v>
       </c>
       <c r="C174" t="s">
         <v>235</v>
@@ -5119,7 +5111,7 @@
       </c>
       <c r="B175" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BYDVQJ</v>
+        <v>LRFNKN</v>
       </c>
       <c r="C175" t="s">
         <v>239</v>
@@ -5146,7 +5138,7 @@
       </c>
       <c r="B176" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FGTPLH</v>
+        <v>KVGLZK</v>
       </c>
       <c r="C176" t="s">
         <v>241</v>
@@ -5176,7 +5168,7 @@
       </c>
       <c r="B177" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VZEJPH</v>
+        <v>RTJFQG</v>
       </c>
       <c r="C177" t="s">
         <v>244</v>
@@ -5206,7 +5198,7 @@
       </c>
       <c r="B178" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NJWHBM</v>
+        <v>WTYHIF</v>
       </c>
       <c r="C178" t="s">
         <v>245</v>
@@ -5227,7 +5219,7 @@
       </c>
       <c r="B179" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YZKGUX</v>
+        <v>GDEBSM</v>
       </c>
       <c r="C179" t="s">
         <v>246</v>
@@ -5248,7 +5240,7 @@
       </c>
       <c r="B180" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ETICUJ</v>
+        <v>KVJGMZ</v>
       </c>
       <c r="C180" t="s">
         <v>323</v>
@@ -5269,7 +5261,7 @@
       </c>
       <c r="B181" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TDYHXX</v>
+        <v>THXJFV</v>
       </c>
       <c r="C181" t="s">
         <v>324</v>
@@ -5290,7 +5282,7 @@
       </c>
       <c r="B182" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CEIXNK</v>
+        <v>SLRZCQ</v>
       </c>
       <c r="C182" t="s">
         <v>325</v>
@@ -5311,7 +5303,7 @@
       </c>
       <c r="B183" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AZRYNB</v>
+        <v>LYITKB</v>
       </c>
       <c r="C183" t="s">
         <v>326</v>
@@ -5332,7 +5324,7 @@
       </c>
       <c r="B184" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DHUOSH</v>
+        <v>EPJRVD</v>
       </c>
       <c r="C184" t="s">
         <v>327</v>
@@ -5353,7 +5345,7 @@
       </c>
       <c r="B185" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZIKQLM</v>
+        <v>URQCXX</v>
       </c>
       <c r="C185" t="s">
         <v>328</v>
@@ -5374,7 +5366,7 @@
       </c>
       <c r="B186" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KDBUQM</v>
+        <v>OJVSOI</v>
       </c>
       <c r="C186" t="s">
         <v>329</v>
@@ -5395,7 +5387,7 @@
       </c>
       <c r="B187" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VIUFJL</v>
+        <v>ACQHWU</v>
       </c>
       <c r="C187" t="s">
         <v>330</v>

</xml_diff>

<commit_message>
xlsx validation added ROUTINE, TAGNAME, ADDR validation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kek\PycharmProjects\RSLogix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EE1C3E-3780-4FF8-BF30-CEF1178227C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DC2F70-439F-4676-A066-88E160160913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10485" yWindow="3240" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1549,8 +1549,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="B2" s="2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>XMHDCO</v>
+        <v>DSJQAR</v>
       </c>
       <c r="C2" t="s">
         <v>332</v>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" ref="B4:B63" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>GTQLBU</v>
+        <v>FUNVZB</v>
       </c>
       <c r="C4" t="s">
         <v>337</v>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>MGBMID</v>
+        <v>KDJGEJ</v>
       </c>
       <c r="C21" t="s">
         <v>360</v>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PZWCFO</v>
+        <v>QOJZVL</v>
       </c>
       <c r="C23" t="s">
         <v>362</v>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>BJLIDE</v>
+        <v>CDFFTP</v>
       </c>
       <c r="C25" t="s">
         <v>364</v>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B27" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>YMSLOP</v>
+        <v>ILFLPE</v>
       </c>
       <c r="C27" t="s">
         <v>366</v>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="B29" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>GATSNU</v>
+        <v>PORCMU</v>
       </c>
       <c r="C29" t="s">
         <v>368</v>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="B31" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>BQSCYY</v>
+        <v>ECOWTS</v>
       </c>
       <c r="C31" t="s">
         <v>370</v>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="B33" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HQYUPV</v>
+        <v>AYJJQR</v>
       </c>
       <c r="C33" t="s">
         <v>375</v>
@@ -2185,7 +2185,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SXHQPN</v>
+        <v>YOVKSI</v>
       </c>
       <c r="C35" t="s">
         <v>376</v>
@@ -2270,7 +2270,7 @@
       </c>
       <c r="B42" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>TAZMPN</v>
+        <v>FTDZES</v>
       </c>
       <c r="C42" t="s">
         <v>252</v>
@@ -2294,7 +2294,7 @@
       </c>
       <c r="B43" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WUECTU</v>
+        <v>XTMOBH</v>
       </c>
       <c r="D43" t="s">
         <v>257</v>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="B44" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>MBXYPM</v>
+        <v>WZLZDX</v>
       </c>
       <c r="D44" t="s">
         <v>259</v>
@@ -2324,7 +2324,7 @@
       </c>
       <c r="B45" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>OPPBUR</v>
+        <v>QWTINK</v>
       </c>
       <c r="C45" t="s">
         <v>261</v>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="B48" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HJEXQN</v>
+        <v>MLHMBG</v>
       </c>
       <c r="C48" t="s">
         <v>267</v>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="B52" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>VZJXOE</v>
+        <v>DUZYOQ</v>
       </c>
       <c r="C52" t="s">
         <v>271</v>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="B57" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DFASJC</v>
+        <v>BLQYQW</v>
       </c>
       <c r="C57" t="s">
         <v>273</v>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="B60" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ZAGWXK</v>
+        <v>MKEVRD</v>
       </c>
       <c r="C60" t="s">
         <v>274</v>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="B63" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>MEMLFH</v>
+        <v>GTTHQE</v>
       </c>
       <c r="C63" t="s">
         <v>275</v>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B67" s="2" t="str">
         <f t="shared" ref="B67:B130" ca="1" si="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>RUPRIB</v>
+        <v>KELIUZ</v>
       </c>
       <c r="C67" t="s">
         <v>276</v>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="B70" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSQGZU</v>
+        <v>NHEMPB</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>10</v>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="B71" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PHBLOO</v>
+        <v>ZISSHB</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>17</v>
@@ -2725,7 +2725,7 @@
       </c>
       <c r="B72" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VVTXPY</v>
+        <v>UWMDYZ</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>23</v>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="B73" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BKRGYH</v>
+        <v>FJAIKR</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>27</v>
@@ -2779,7 +2779,7 @@
       </c>
       <c r="B74" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>COKYOB</v>
+        <v>NHAPPF</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>33</v>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="B75" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JDRHBD</v>
+        <v>ACYHSK</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>37</v>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="B76" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HAMIDS</v>
+        <v>GEYELQ</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>41</v>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B77" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WAPGQM</v>
+        <v>KIFQEF</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>46</v>
@@ -2884,7 +2884,7 @@
       </c>
       <c r="B78" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XUWFSB</v>
+        <v>KJJFBT</v>
       </c>
       <c r="C78" t="s">
         <v>138</v>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="B79" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NGTSHU</v>
+        <v>QZFRON</v>
       </c>
       <c r="C79" t="s">
         <v>140</v>
@@ -2938,7 +2938,7 @@
       </c>
       <c r="B80" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GVNSQE</v>
+        <v>JBFPEV</v>
       </c>
       <c r="C80" t="s">
         <v>142</v>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="B81" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UFLXOM</v>
+        <v>ZRIGHU</v>
       </c>
       <c r="C81" t="s">
         <v>144</v>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="B82" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VOOACM</v>
+        <v>NIJFJF</v>
       </c>
       <c r="C82" t="s">
         <v>147</v>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="B83" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JULOUS</v>
+        <v>CZBOWN</v>
       </c>
       <c r="C83" t="s">
         <v>148</v>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B84" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LBMTYJ</v>
+        <v>LZIJPX</v>
       </c>
       <c r="C84" t="s">
         <v>152</v>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="B85" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TKAHFW</v>
+        <v>RQNFJO</v>
       </c>
       <c r="C85" t="s">
         <v>154</v>
@@ -3098,7 +3098,7 @@
       </c>
       <c r="B87" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZCZNPS</v>
+        <v>XJFEEY</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>51</v>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="B88" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BVPRPY</v>
+        <v>VSISCW</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>53</v>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="B89" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ABVQQP</v>
+        <v>RRRUHX</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>57</v>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="B90" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CILYNR</v>
+        <v>SVIPXJ</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>60</v>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="B91" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BXQCZD</v>
+        <v>SHBBJI</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>63</v>
@@ -3221,7 +3221,7 @@
       </c>
       <c r="B92" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FHZIGI</v>
+        <v>GDMCRN</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>65</v>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="B93" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HXQMWL</v>
+        <v>TOOZYW</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>68</v>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="B94" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VEHMOP</v>
+        <v>WONSNQ</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>70</v>
@@ -3293,7 +3293,7 @@
       </c>
       <c r="B95" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INREMB</v>
+        <v>WVTIJV</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>73</v>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="B96" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IKEXJS</v>
+        <v>SWFODJ</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>77</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B97" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BFSEXX</v>
+        <v>OOLATG</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>81</v>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="B98" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CLGBSA</v>
+        <v>DRFMYQ</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>85</v>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="B99" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GQETJU</v>
+        <v>OYPCLO</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>89</v>
@@ -3413,7 +3413,7 @@
       </c>
       <c r="B100" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JHKAJZ</v>
+        <v>IQWAPL</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>93</v>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="B101" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LIBIVB</v>
+        <v>CCBLKK</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>99</v>
@@ -3470,7 +3470,7 @@
       </c>
       <c r="B102" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BRETEF</v>
+        <v>EJBYUT</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>106</v>
@@ -3505,7 +3505,7 @@
       </c>
       <c r="B104" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>RMNRTG</v>
+        <v>YTQEZX</v>
       </c>
       <c r="C104" t="s">
         <v>114</v>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="B105" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TDEMSK</v>
+        <v>LTOVQE</v>
       </c>
       <c r="C105" t="s">
         <v>117</v>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="B106" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VDJTHW</v>
+        <v>QXYNTV</v>
       </c>
       <c r="C106" t="s">
         <v>120</v>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="B107" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DXACVQ</v>
+        <v>AODTWQ</v>
       </c>
       <c r="C107" t="s">
         <v>123</v>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="B108" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XILBQY</v>
+        <v>IJNPXJ</v>
       </c>
       <c r="C108" t="s">
         <v>126</v>
@@ -3625,7 +3625,7 @@
       </c>
       <c r="B109" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GHECNY</v>
+        <v>UIQVGN</v>
       </c>
       <c r="C109" t="s">
         <v>129</v>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="B110" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KGWQYZ</v>
+        <v>NWRNQR</v>
       </c>
       <c r="C110" t="s">
         <v>132</v>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="B111" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HNRZXF</v>
+        <v>EEOBWP</v>
       </c>
       <c r="C111" t="s">
         <v>135</v>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="B112" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GPIAQL</v>
+        <v>ACEFVG</v>
       </c>
       <c r="C112" t="s">
         <v>158</v>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="B113" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HZMSJS</v>
+        <v>GQUEWD</v>
       </c>
       <c r="C113" t="s">
         <v>162</v>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="B114" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>RFGQLA</v>
+        <v>NUGZQP</v>
       </c>
       <c r="C114" t="s">
         <v>164</v>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="B115" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZKYBXN</v>
+        <v>ZBNKEM</v>
       </c>
       <c r="C115" t="s">
         <v>168</v>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="B116" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VPPRNO</v>
+        <v>GASZYD</v>
       </c>
       <c r="C116" t="s">
         <v>169</v>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="B117" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LBATSL</v>
+        <v>UYOMKN</v>
       </c>
       <c r="C117" t="s">
         <v>171</v>
@@ -3847,7 +3847,7 @@
       </c>
       <c r="B118" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OPZSAF</v>
+        <v>SBUEGJ</v>
       </c>
       <c r="C118" t="s">
         <v>172</v>
@@ -3868,7 +3868,7 @@
       </c>
       <c r="B119" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QBHCCV</v>
+        <v>SYZEHQ</v>
       </c>
       <c r="C119" t="s">
         <v>173</v>
@@ -3896,7 +3896,7 @@
       </c>
       <c r="B121" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HYLLFY</v>
+        <v>GGZPUC</v>
       </c>
       <c r="C121" t="s">
         <v>278</v>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="B122" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CQJTSW</v>
+        <v>GYMLPK</v>
       </c>
       <c r="C122" t="s">
         <v>281</v>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="B123" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ULHQPR</v>
+        <v>IDBVMQ</v>
       </c>
       <c r="C123" t="s">
         <v>284</v>
@@ -3968,7 +3968,7 @@
       </c>
       <c r="B124" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HIZTDM</v>
+        <v>KMPXZM</v>
       </c>
       <c r="C124" t="s">
         <v>287</v>
@@ -3992,7 +3992,7 @@
       </c>
       <c r="B125" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IWVOUK</v>
+        <v>JUNDUC</v>
       </c>
       <c r="C125" t="s">
         <v>290</v>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="B126" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>YZHPZP</v>
+        <v>RCXBFZ</v>
       </c>
       <c r="C126" t="s">
         <v>292</v>
@@ -4040,7 +4040,7 @@
       </c>
       <c r="B127" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VBZCBP</v>
+        <v>CRWZVP</v>
       </c>
       <c r="C127" t="s">
         <v>294</v>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="B128" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>YKEFCZ</v>
+        <v>BGUYAH</v>
       </c>
       <c r="C128" t="s">
         <v>296</v>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="B129" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QNBRST</v>
+        <v>IOUJYB</v>
       </c>
       <c r="C129" t="s">
         <v>298</v>
@@ -4112,7 +4112,7 @@
       </c>
       <c r="B130" s="2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>EOWHGO</v>
+        <v>LTTDNZ</v>
       </c>
       <c r="C130" t="s">
         <v>300</v>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="B131" s="2" t="str">
         <f t="shared" ref="B131:B187" ca="1" si="2">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>WDAJPW</v>
+        <v>JROPNU</v>
       </c>
       <c r="C131" t="s">
         <v>302</v>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="B132" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HZHELH</v>
+        <v>PYHMGT</v>
       </c>
       <c r="C132" t="s">
         <v>304</v>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="B133" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NRDYZQ</v>
+        <v>QGFWTJ</v>
       </c>
       <c r="C133" t="s">
         <v>306</v>
@@ -4208,7 +4208,7 @@
       </c>
       <c r="B134" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WBBJZY</v>
+        <v>SIYJTD</v>
       </c>
       <c r="C134" t="s">
         <v>308</v>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="B135" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WEQLCL</v>
+        <v>QEHOIU</v>
       </c>
       <c r="C135" t="s">
         <v>309</v>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="B136" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>EICODP</v>
+        <v>JZTIUK</v>
       </c>
       <c r="C136" t="s">
         <v>310</v>
@@ -4284,7 +4284,7 @@
       </c>
       <c r="B138" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NUAVWM</v>
+        <v>KZPUXC</v>
       </c>
       <c r="C138" t="s">
         <v>312</v>
@@ -4308,7 +4308,7 @@
       </c>
       <c r="B139" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RFTCPP</v>
+        <v>JAODRF</v>
       </c>
       <c r="C139" t="s">
         <v>313</v>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="B140" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HFWDNA</v>
+        <v>RJGWVP</v>
       </c>
       <c r="C140" t="s">
         <v>314</v>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="B141" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YBUKUE</v>
+        <v>WXSTPA</v>
       </c>
       <c r="C141" t="s">
         <v>315</v>
@@ -4380,7 +4380,7 @@
       </c>
       <c r="B142" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TNOHFS</v>
+        <v>NKVFOY</v>
       </c>
       <c r="C142" t="s">
         <v>316</v>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="B143" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LVAFZQ</v>
+        <v>BTYMLT</v>
       </c>
       <c r="C143" t="s">
         <v>317</v>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="B144" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HQNNPT</v>
+        <v>ZPPZME</v>
       </c>
       <c r="C144" t="s">
         <v>319</v>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="B145" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LCVEIY</v>
+        <v>HIGBCI</v>
       </c>
       <c r="C145" t="s">
         <v>321</v>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="B146" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JBHUJX</v>
+        <v>ZPVXTX</v>
       </c>
       <c r="C146" t="s">
         <v>377</v>
@@ -4500,7 +4500,7 @@
       </c>
       <c r="B147" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QKLTAO</v>
+        <v>BANUQM</v>
       </c>
       <c r="C147" t="s">
         <v>379</v>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="B148" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>IOEICW</v>
+        <v>QTBSXV</v>
       </c>
       <c r="C148" t="s">
         <v>381</v>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="B149" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HSVDRP</v>
+        <v>OYMECK</v>
       </c>
       <c r="C149" t="s">
         <v>382</v>
@@ -4563,7 +4563,7 @@
       </c>
       <c r="B150" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DJUMYY</v>
+        <v>IDUUKK</v>
       </c>
       <c r="C150" t="s">
         <v>383</v>
@@ -4584,7 +4584,7 @@
       </c>
       <c r="B151" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FMZJFL</v>
+        <v>DRSPKI</v>
       </c>
       <c r="C151" t="s">
         <v>384</v>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="B152" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CWOONP</v>
+        <v>UNLBIL</v>
       </c>
       <c r="C152" t="s">
         <v>385</v>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="B153" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RYZPBK</v>
+        <v>PRGDEY</v>
       </c>
       <c r="C153" t="s">
         <v>386</v>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="B155" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YZNULD</v>
+        <v>NVECPW</v>
       </c>
       <c r="C155" t="s">
         <v>177</v>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="B156" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OOPKOA</v>
+        <v>LOAYNW</v>
       </c>
       <c r="C156" t="s">
         <v>183</v>
@@ -4708,7 +4708,7 @@
       </c>
       <c r="B157" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HBYDHD</v>
+        <v>TJYGCB</v>
       </c>
       <c r="C157" t="s">
         <v>188</v>
@@ -4735,7 +4735,7 @@
       </c>
       <c r="B158" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HPSPXC</v>
+        <v>GMUEQN</v>
       </c>
       <c r="C158" t="s">
         <v>192</v>
@@ -4762,7 +4762,7 @@
       </c>
       <c r="B159" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TTCMVV</v>
+        <v>NSRVYD</v>
       </c>
       <c r="C159" t="s">
         <v>196</v>
@@ -4789,7 +4789,7 @@
       </c>
       <c r="B160" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NRSCIN</v>
+        <v>WMGVHK</v>
       </c>
       <c r="C160" t="s">
         <v>200</v>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="B161" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>EPMRUY</v>
+        <v>WEDZWO</v>
       </c>
       <c r="C161" t="s">
         <v>204</v>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="B162" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PFPVCC</v>
+        <v>JLFABM</v>
       </c>
       <c r="C162" t="s">
         <v>207</v>
@@ -4858,7 +4858,7 @@
       </c>
       <c r="B163" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NDGMLP</v>
+        <v>PVYZGP</v>
       </c>
       <c r="C163" t="s">
         <v>210</v>
@@ -4879,7 +4879,7 @@
       </c>
       <c r="B164" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QMQJJR</v>
+        <v>OYMCWY</v>
       </c>
       <c r="C164" t="s">
         <v>213</v>
@@ -4900,7 +4900,7 @@
       </c>
       <c r="B165" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FATZIB</v>
+        <v>BPWNQH</v>
       </c>
       <c r="C165" t="s">
         <v>216</v>
@@ -4921,7 +4921,7 @@
       </c>
       <c r="B166" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RWHSMY</v>
+        <v>JYUNMA</v>
       </c>
       <c r="C166" t="s">
         <v>219</v>
@@ -4942,7 +4942,7 @@
       </c>
       <c r="B167" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XJMXPT</v>
+        <v>SZZDAG</v>
       </c>
       <c r="C167" t="s">
         <v>222</v>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="B168" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PUXSZK</v>
+        <v>EDJYYA</v>
       </c>
       <c r="C168" t="s">
         <v>224</v>
@@ -4984,7 +4984,7 @@
       </c>
       <c r="B169" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FEJJMC</v>
+        <v>EZFUHV</v>
       </c>
       <c r="C169" t="s">
         <v>226</v>
@@ -5008,7 +5008,7 @@
       </c>
       <c r="B170" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KGCANG</v>
+        <v>BWMWWV</v>
       </c>
       <c r="C170" t="s">
         <v>229</v>
@@ -5036,7 +5036,7 @@
       </c>
       <c r="B172" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VDDUWL</v>
+        <v>MFVQXL</v>
       </c>
       <c r="C172" t="s">
         <v>232</v>
@@ -5060,7 +5060,7 @@
       </c>
       <c r="B173" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ULLRJF</v>
+        <v>AQXZOO</v>
       </c>
       <c r="C173" t="s">
         <v>233</v>
@@ -5084,7 +5084,7 @@
       </c>
       <c r="B174" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XAEQIJ</v>
+        <v>PLNJKU</v>
       </c>
       <c r="C174" t="s">
         <v>235</v>
@@ -5111,7 +5111,7 @@
       </c>
       <c r="B175" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LRFNKN</v>
+        <v>BZIXTJ</v>
       </c>
       <c r="C175" t="s">
         <v>239</v>
@@ -5138,7 +5138,7 @@
       </c>
       <c r="B176" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KVGLZK</v>
+        <v>VYAGAT</v>
       </c>
       <c r="C176" t="s">
         <v>241</v>
@@ -5168,7 +5168,7 @@
       </c>
       <c r="B177" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RTJFQG</v>
+        <v>VDSLMP</v>
       </c>
       <c r="C177" t="s">
         <v>244</v>
@@ -5198,7 +5198,7 @@
       </c>
       <c r="B178" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WTYHIF</v>
+        <v>QJVHVJ</v>
       </c>
       <c r="C178" t="s">
         <v>245</v>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="B179" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GDEBSM</v>
+        <v>YISOBX</v>
       </c>
       <c r="C179" t="s">
         <v>246</v>
@@ -5240,7 +5240,7 @@
       </c>
       <c r="B180" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KVJGMZ</v>
+        <v>OXTQFJ</v>
       </c>
       <c r="C180" t="s">
         <v>323</v>
@@ -5261,7 +5261,7 @@
       </c>
       <c r="B181" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>THXJFV</v>
+        <v>MFRBBS</v>
       </c>
       <c r="C181" t="s">
         <v>324</v>
@@ -5282,7 +5282,7 @@
       </c>
       <c r="B182" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SLRZCQ</v>
+        <v>KICPVW</v>
       </c>
       <c r="C182" t="s">
         <v>325</v>
@@ -5303,7 +5303,7 @@
       </c>
       <c r="B183" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LYITKB</v>
+        <v>SOGKDN</v>
       </c>
       <c r="C183" t="s">
         <v>326</v>
@@ -5324,7 +5324,7 @@
       </c>
       <c r="B184" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>EPJRVD</v>
+        <v>RMKVBF</v>
       </c>
       <c r="C184" t="s">
         <v>327</v>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="B185" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>URQCXX</v>
+        <v>UESRBT</v>
       </c>
       <c r="C185" t="s">
         <v>328</v>
@@ -5366,7 +5366,7 @@
       </c>
       <c r="B186" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OJVSOI</v>
+        <v>ATFXEU</v>
       </c>
       <c r="C186" t="s">
         <v>329</v>
@@ -5387,7 +5387,7 @@
       </c>
       <c r="B187" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ACQHWU</v>
+        <v>YBXENE</v>
       </c>
       <c r="C187" t="s">
         <v>330</v>

</xml_diff>